<commit_message>
Add Bayesian estimation scripts and visualizations
- Implemented GGG_bayesian_B.py and GGG_bayesian_H.py for Bayesian estimation of magnetic susceptibility.
- Added verification script verify_chi_calculation.py to validate susceptibility calculations.
- Created exp_plt.py for plotting experimental data.
- Generated trace plots and fitting result images (B_trace_plot.png, B_fitting_result.png, H_trace_plot.png, H_fitting_result.png).
- Added workflow_detailed for visual representation of the Bayesian estimation process.
- Included new Excel data file Circular_Polarization_B_Field.xlsx for analysis.
- Removed obsolete test2.py script and unnecessary images.
</commit_message>
<xml_diff>
--- a/Circular_Polarization_B_Field.xlsx
+++ b/Circular_Polarization_B_Field.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ynuoffice365-my.sharepoint.com/personal/nakao-taichi-ph_ynu_jp/Documents/修士/磁性/GGG/Programs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="70" documentId="8_{912145C6-2774-4C3F-81FA-9E7FFD5DE2F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8FD7D0D9-4D42-4CE0-A533-B823CF47B8ED}"/>
+  <xr:revisionPtr revIDLastSave="75" documentId="8_{912145C6-2774-4C3F-81FA-9E7FFD5DE2F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6BBC331E-0318-4D39-BDBC-D1AF2819E91C}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{9970D8DA-C067-4AF6-B4A1-755CFF5BCC47}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{9970D8DA-C067-4AF6-B4A1-755CFF5BCC47}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22230,7 +22230,1397 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ja-JP"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ja-JP"/>
+              <a:t>B = 7.8 T, T= * K</a:t>
+            </a:r>
+            <a:endParaRPr lang="ja-JP" altLang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ja-JP"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$2:$A$175</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="174"/>
+                <c:pt idx="0">
+                  <c:v>0.15144113336590101</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.15632633121641401</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.16121152906692701</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.16609672691744001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.17098192476795299</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.17586712261846599</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.18075232046897799</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.18563751831949099</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.19052271617000399</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.19540791402051699</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.20029311187102999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.205178309721543</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.210063507572056</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.214948705422569</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.219833903273082</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.224719101123595</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.229604298974108</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.234489496824621</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.239374694675134</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.244259892525647</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.24914509037616001</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.25403028822667301</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.25891548607718601</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.26380068392769901</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.26868588177821201</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.27357107962872401</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.27845627747923701</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.28334147532975001</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.28822667318026302</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.29311187103077602</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.29799706888128902</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.30288226673180202</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.30776746458231502</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.31265266243282802</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.31753786028334102</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.32242305813385402</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.32730825598436702</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.33219345383488003</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.33707865168539303</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.34196384953590597</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.34684904738641897</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.35173424523693197</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.35661944308744498</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.36150464093795698</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.36638983878846998</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.37127503663898298</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.37616023448949598</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.38104543234000898</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.38593063019052198</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.39081582804103498</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.39570102589154799</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.40058622374206099</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.40547142159257399</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.41035661944308699</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.41524181729359999</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.42012701514411299</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.42501221299462599</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.42989741084513899</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.434782608695652</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.439667806546165</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.444553004396678</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.44943820224719</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.454323400097703</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.459208597948216</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.464093795798729</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.468978993649242</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.47386419149975501</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.47874938935026801</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.48363458720078101</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.48851978505129401</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.49340498290180701</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.49829018075232001</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.50317537860283301</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.50806057645334601</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.51294577430385901</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.51783097215437202</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.52271617000488502</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.52760136785539802</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.53248656570591102</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.53737176355642402</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.54225696140693702</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.54714215925744902</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0.55202735710796202</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.55691255495847503</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.56179775280898803</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0.56668295065950103</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.57156814851001403</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0.57645334636052703</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0.58133854421104003</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0.58622374206155303</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0.59110893991206603</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0.59599413776257903</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0.60087933561309204</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0.60576453346360504</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0.61064973131411804</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0.61553492916463104</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0.62042012701514404</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0.62530532486565704</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0.63019052271616904</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>0.63507572056668204</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>0.63996091841719505</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>0.64484611626770805</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>0.64973131411822105</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>0.65461651196873405</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>0.65950170981924705</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>0.66438690766976005</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>0.66927210552027305</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>0.67415730337078605</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>0.67904250122129906</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>0.68392769907181195</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>0.68881289692232495</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>0.69369809477283795</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>0.69858329262335095</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>0.70346849047386395</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>0.70835368832437695</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>0.71323888617488995</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>0.71812408402540295</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>0.72300928187591496</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>0.72789447972642796</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>0.73277967757694096</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>0.73766487542745396</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>0.74255007327796696</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>0.74743527112847996</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>0.75232046897899296</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>0.75720566682950596</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>0.76209086468001896</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>0.76697606253053197</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>0.77186126038104497</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>0.77674645823155797</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>0.78163165608207097</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>0.78651685393258397</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>0.79140205178309697</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>0.79628724963360997</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>0.80117244748412297</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>0.80605764533463498</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>0.81094284318514798</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>0.81582804103566098</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>0.82071323888617398</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>0.82559843673668698</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>0.83048363458719998</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>0.83536883243771298</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>0.84025403028822598</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>0.84513922813873898</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>0.85002442598925199</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>0.85490962383976499</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>0.85979482169027799</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>0.86468001954079099</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>0.86956521739130399</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>0.87445041524181699</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>0.87933561309232999</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>0.88422081094284299</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>0.889106008793356</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>0.893991206643869</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>0.898876404494381</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>0.903761602344894</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>0.908646800195407</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>0.91353199804592</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>0.918417195896433</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>0.923302393746946</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>0.92818759159745901</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>0.93307278944797201</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>0.93795798729848501</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>0.94284318514899801</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>0.94772838299951101</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>0.95261358085002401</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>0.95749877870053701</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>0.96238397655105001</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>0.96726917440156301</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>0.97215437225207602</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>0.97703957010258902</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>0.98192476795310202</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>0.98680996580361502</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>0.99169516365412802</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>0.99658036150464002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$B$2:$B$175</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="174"/>
+                <c:pt idx="0">
+                  <c:v>3.5827409132350399E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.6051715854411803E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.40476108790587E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0119816798053801E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.4924490685152501E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.9220520266884401E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.3692133846826901E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.8587925672797795E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.0477714574850901E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.3979883086922798E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.7617719986829803E-4</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.0365317506685498E-4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.0337663426309202E-4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8.74550563877899E-4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.4833338142009999E-3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.1365960733806901E-3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.90466213510612E-3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.9858358834371803E-3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5.6367101099400897E-3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>8.1008996263599205E-3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.15547255896546E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.60705545379424E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.1590827392319802E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.7909242697055199E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.4664505899412598E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>4.1359756110880497E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4.7420361966253301E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>5.2289585372559302E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>5.5539301570066299E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>5.6956463666557197E-2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>5.6571474391119099E-2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>5.4621907045080999E-2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>5.1474554444028098E-2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>4.7540517399910699E-2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>4.3209367068586003E-2</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3.8811372559739397E-2</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>3.4603569317723397E-2</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>3.0770296038464099E-2</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2.74298070493833E-2</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2.4642157101021901E-2</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2.2417139082220702E-2</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2.0723209382903E-2</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1.94985688892572E-2</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1.8664283597402902E-2</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1.8137690604939499E-2</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1.7843583875003399E-2</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1.7721265518117001E-2</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1.77269454481747E-2</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1.7832267250290499E-2</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1.8020393090541001E-2</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1.8281136198591001E-2</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1.8606421241686599E-2</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1.8987142798445902E-2</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1.94122886490538E-2</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1.98708091807102E-2</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>2.0355999007788301E-2</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>2.0871266852844898E-2</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>2.1435575622178599E-2</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>2.2086950005036299E-2</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>2.2883189570739801E-2</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>2.3899725800537099E-2</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>2.5224882636675699E-2</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>2.6952584380212401E-2</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>2.91722238457164E-2</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>3.1955531197356599E-2</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>3.5341242412314698E-2</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>3.9320045032680197E-2</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>4.3823903919322997E-2</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>4.8724167414664503E-2</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>5.3840834551512298E-2</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>5.8961410632371203E-2</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>6.3863941324877702E-2</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>6.8337515855273701E-2</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>7.2195605670122301E-2</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>7.5281655292373503E-2</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>7.7469981282800901E-2</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>7.8666600634977393E-2</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>7.8813785035292905E-2</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>7.7899509918493898E-2</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>7.5969501107572598E-2</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>7.3136532879293198E-2</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>6.9580529152040702E-2</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>6.55350571192298E-2</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>6.1260695483762201E-2</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>5.7011224246728102E-2</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>5.3001547194189903E-2</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>4.9385144462634402E-2</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>4.6244753859428202E-2</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>4.3595548987426701E-2</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>4.1397402136849101E-2</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>3.9572269173285997E-2</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>3.8023410335511799E-2</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>3.6653967440295601E-2</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>3.5382830305137003E-2</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>3.4155915830007301E-2</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>3.2951449173450199E-2</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>3.1778865197959298E-2</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>3.06723072331503E-2</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>2.96807900176622E-2</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>2.88574238833403E-2</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>2.8249648815600801E-2</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>2.7891608962568901E-2</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>2.7799108726854399E-2</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>2.7967302505585202E-2</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>2.83713233544261E-2</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>2.8970153178562101E-2</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>2.9713832720817498E-2</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>3.0553436519060201E-2</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>3.1452277454919901E-2</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>3.2396054560192601E-2</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>3.3399620805594499E-2</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>3.4508836268559599E-2</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>3.57971776339608E-2</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>3.7357776050675098E-2</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>3.9291993957758599E-2</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>4.1695656235142799E-2</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>4.4644061315665597E-2</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>4.8177277508122701E-2</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>5.2287940877640403E-2</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>5.6914293668251598E-2</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>6.1940799558465799E-2</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>6.7206954344707706E-2</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>7.2522352549166197E-2</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>7.7683947699235506E-2</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>8.2491026880265106E-2</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>8.6755027114146205E-2</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>9.0304094656402101E-2</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>9.2984848397543396E-2</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>9.4665093364769304E-2</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>9.5240842872494499E-2</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>9.4649072048724997E-2</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>9.2884611774852702E-2</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>9.0016389292825905E-2</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>8.6196218509953099E-2</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>8.1654007363292799E-2</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>7.6677079009575794E-2</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>7.1576921730843499E-2</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>6.6651259353836104E-2</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>6.2150451604517799E-2</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>5.8254650878065702E-2</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>5.5063788636603002E-2</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>5.25988021127064E-2</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>5.08108980294011E-2</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>4.9595922118596397E-2</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>4.8812005952147297E-2</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>4.8299495147202699E-2</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>4.7902124349807999E-2</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>4.7487575743993697E-2</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>4.6964591987756897E-2</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>4.62935561146317E-2</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>4.5488398752471397E-2</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>4.4609624501594697E-2</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>4.3750333737472703E-2</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>4.3018472032911897E-2</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>4.2518786817037503E-2</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>4.2337351861983702E-2</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>4.25305828165813E-2</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>4.3119847651605502E-2</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>4.4092185191317697E-2</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>4.54071211917913E-2</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>4.7008885522450403E-2</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>4.8842397019463503E-2</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>5.0870351608130998E-2</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>5.3087984816479097E-2</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>5.5531975710647399E-2</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>5.8280734703072899E-2</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>6.1444886660612902E-2</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>6.5148748568617507E-2</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>6.9505486005533801E-2</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>7.4589932279074705E-2</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>8.04134797046476E-2</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>8.6904994359812707E-2</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>9.3900628313456899E-2</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>0.101144138678887</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5DC4-442F-AE22-94D4B96681BA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1261120975"/>
+        <c:axId val="1261118095"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1261120975"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ja-JP"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1261118095"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1261118095"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ja-JP"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1261120975"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ja-JP"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -22786,6 +24176,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -22807,6 +24713,47 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1883707F-FCDE-A27A-B89B-8C883FB9A97A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>439615</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>146539</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>160338</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="グラフ 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20BC4880-66CF-5BDA-3723-E06500008433}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -34539,8 +36486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DADCFAAC-AB09-4CA6-B1FF-A237551E8235}">
   <dimension ref="A1:B175"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="Z8" sqref="Z8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -35948,6 +37895,7 @@
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>